<commit_message>
Add new_korr and some edits
</commit_message>
<xml_diff>
--- a/eff.xlsx
+++ b/eff.xlsx
@@ -441,22 +441,22 @@
         <v>4</v>
       </c>
       <c r="C1" t="n">
-        <v>1.48</v>
+        <v>1.75</v>
       </c>
       <c r="D1" t="n">
-        <v>1.91</v>
+        <v>2.08</v>
       </c>
       <c r="E1" t="n">
-        <v>3.46</v>
+        <v>2.24</v>
       </c>
       <c r="F1" t="n">
-        <v>4.1</v>
+        <v>2.21</v>
       </c>
       <c r="G1" t="n">
-        <v>4.56</v>
+        <v>2.23</v>
       </c>
       <c r="H1" t="n">
-        <v>4.8</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="2">
@@ -467,22 +467,22 @@
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>1.53</v>
+        <v>1.55</v>
       </c>
       <c r="D2" t="n">
         <v>2.31</v>
       </c>
       <c r="E2" t="n">
-        <v>4.39</v>
+        <v>2.29</v>
       </c>
       <c r="F2" t="n">
-        <v>5.62</v>
+        <v>2.32</v>
       </c>
       <c r="G2" t="n">
-        <v>6.07</v>
+        <v>2.31</v>
       </c>
       <c r="H2" t="n">
-        <v>6.25</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="3">
@@ -493,22 +493,22 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>1.81</v>
+        <v>1.89</v>
       </c>
       <c r="D3" t="n">
-        <v>2.84</v>
+        <v>2.38</v>
       </c>
       <c r="E3" t="n">
-        <v>4.6</v>
+        <v>2.37</v>
       </c>
       <c r="F3" t="n">
-        <v>6.86</v>
+        <v>2.38</v>
       </c>
       <c r="G3" t="n">
-        <v>8.029999999999999</v>
+        <v>2.37</v>
       </c>
       <c r="H3" t="n">
-        <v>8.710000000000001</v>
+        <v>2.37</v>
       </c>
     </row>
     <row r="4">
@@ -519,22 +519,22 @@
         <v>7</v>
       </c>
       <c r="C4" t="n">
-        <v>1.95</v>
+        <v>1.49</v>
       </c>
       <c r="D4" t="n">
-        <v>2.99</v>
+        <v>2.47</v>
       </c>
       <c r="E4" t="n">
-        <v>6.42</v>
+        <v>2.46</v>
       </c>
       <c r="F4" t="n">
-        <v>9.039999999999999</v>
+        <v>2.48</v>
       </c>
       <c r="G4" t="n">
-        <v>11.14</v>
+        <v>2.47</v>
       </c>
       <c r="H4" t="n">
-        <v>11.57</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="5">
@@ -545,22 +545,22 @@
         <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>2.13</v>
+        <v>2.3</v>
       </c>
       <c r="D5" t="n">
-        <v>3.57</v>
+        <v>2.53</v>
       </c>
       <c r="E5" t="n">
-        <v>7.87</v>
+        <v>2.52</v>
       </c>
       <c r="F5" t="n">
-        <v>12.03</v>
+        <v>2.53</v>
       </c>
       <c r="G5" t="n">
-        <v>14.69</v>
+        <v>2.51</v>
       </c>
       <c r="H5" t="n">
-        <v>15.62</v>
+        <v>2.51</v>
       </c>
     </row>
     <row r="6">
@@ -571,22 +571,22 @@
         <v>9</v>
       </c>
       <c r="C6" t="n">
-        <v>2.29</v>
+        <v>1.87</v>
       </c>
       <c r="D6" t="n">
-        <v>4.99</v>
+        <v>2.62</v>
       </c>
       <c r="E6" t="n">
-        <v>10.07</v>
+        <v>2.58</v>
       </c>
       <c r="F6" t="n">
-        <v>17.26</v>
+        <v>2.56</v>
       </c>
       <c r="G6" t="n">
-        <v>20.1</v>
+        <v>2.58</v>
       </c>
       <c r="H6" t="n">
-        <v>21.07</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="7">
@@ -597,22 +597,22 @@
         <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>3.15</v>
+        <v>2.06</v>
       </c>
       <c r="D7" t="n">
-        <v>5.07</v>
+        <v>2.72</v>
       </c>
       <c r="E7" t="n">
-        <v>13.68</v>
+        <v>2.71</v>
       </c>
       <c r="F7" t="n">
-        <v>22.19</v>
+        <v>2.71</v>
       </c>
       <c r="G7" t="n">
-        <v>26.64</v>
+        <v>2.72</v>
       </c>
       <c r="H7" t="n">
-        <v>29.42</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="8">
@@ -623,22 +623,22 @@
         <v>11</v>
       </c>
       <c r="C8" t="n">
-        <v>2.66</v>
+        <v>2.48</v>
       </c>
       <c r="D8" t="n">
-        <v>5.26</v>
+        <v>2.61</v>
       </c>
       <c r="E8" t="n">
-        <v>17.88</v>
+        <v>2.75</v>
       </c>
       <c r="F8" t="n">
-        <v>31.35</v>
+        <v>2.78</v>
       </c>
       <c r="G8" t="n">
-        <v>39.97</v>
+        <v>2.79</v>
       </c>
       <c r="H8" t="n">
-        <v>39.56</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="9">
@@ -649,22 +649,22 @@
         <v>12</v>
       </c>
       <c r="C9" t="n">
-        <v>3.01</v>
+        <v>2.53</v>
       </c>
       <c r="D9" t="n">
-        <v>7.2</v>
+        <v>2.88</v>
       </c>
       <c r="E9" t="n">
-        <v>22.06</v>
+        <v>2.78</v>
       </c>
       <c r="F9" t="n">
-        <v>36.78</v>
+        <v>2.85</v>
       </c>
       <c r="G9" t="n">
-        <v>54.74</v>
+        <v>2.85</v>
       </c>
       <c r="H9" t="n">
-        <v>60.62</v>
+        <v>2.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>